<commit_message>
refactor test code to use fixture for setup and teardown.
Pass test:
1. test_user_can_login_and_logout(admin, clinic staff, doctor, not existed account).
2. test_user_can_see_dashboard(admin, clinic staff, doctor, not existed account).
3. test_patient_list_page(clinic staff).

Next: To add more functional tests.

Another additional code is:
1. add Patient dataclass in config, so that easier to add patient for testing.
</commit_message>
<xml_diff>
--- a/functional-test/test_cases.xlsx
+++ b/functional-test/test_cases.xlsx
@@ -20,9 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
-  <si>
-    <t xml:space="preserve">Clinic Mangement System Functional Test Cases</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
+  <si>
+    <t xml:space="preserve">Clinic Mangement System Functional Test Cases (http://localhost:8000)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Script : django-cms/functional-test/</t>
   </si>
   <si>
     <t xml:space="preserve">No</t>
@@ -31,6 +34,9 @@
     <t xml:space="preserve">Description</t>
   </si>
   <si>
+    <t xml:space="preserve">Test Steps</t>
+  </si>
+  <si>
     <t xml:space="preserve">Test Data</t>
   </si>
   <si>
@@ -44,6 +50,9 @@
   </si>
   <si>
     <t xml:space="preserve">Pass/Fail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verified user can login into the system with valid account (admin)</t>
   </si>
   <si>
     <t xml:space="preserve">1. Login with valid username and password (admin account).
@@ -62,10 +71,13 @@
     <t xml:space="preserve">Admin can login with valid username and password, see welcome message and nav button with Admin written.</t>
   </si>
   <si>
-    <t xml:space="preserve">test_admin_can_login_and_logout</t>
+    <t xml:space="preserve">test_user_can_login_and_logout</t>
   </si>
   <si>
     <t xml:space="preserve">Pass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verified user can login into the system with valid account (staff)</t>
   </si>
   <si>
     <t xml:space="preserve">1. Login with valid username and password (Clinic Staff Account).
@@ -84,7 +96,7 @@
     <t xml:space="preserve">Clinic Staff can login with valid username and password, see welcome message and nav button with Staff1 written.</t>
   </si>
   <si>
-    <t xml:space="preserve">test_clinic_staff_can_login_and_logout</t>
+    <t xml:space="preserve">Verified user can login into the system with valid account (doctor)</t>
   </si>
   <si>
     <t xml:space="preserve">1. Login with valid username and password (Doctor account).
@@ -103,7 +115,81 @@
     <t xml:space="preserve">Doctor can login with valid username and password, see welcome message and nav button with Doctor1 written.</t>
   </si>
   <si>
-    <t xml:space="preserve">test_doctor_can_login_and_logout</t>
+    <t xml:space="preserve">Verified that user with non valid account can’t login into the system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Login with invalid username and password (Non-register Account).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Username: not_existed
+Password: never_registered</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User should not be able to login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User see error messages “Please enter a correct username and password. Note that both fields may be case-sensitive.”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verified that logged in user can see dashboard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. User logged in website with verified account.
+2. User can see “Clinic Management System”.
+3. User can see three button:
+    1. Patient List
+    2. Appointment List
+    3. Check-In List</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Logged in user should be able to see “Clinic Management System” header on the website.
+2. Logged in user should be able to see three button which is Patient List, Appointment List and Check-In List</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. User can see “Clinic Management System” header on the website.
+2. User can see three button which is Patient List, Appointment List and Check-In List.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_user_can_see_dashboard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Verified that logged in user can click on Patient List button and redirect to Patient List page.
+2. Verified that logged in user can see search input with “Search patient” placeholder, and Search button.
+3. Verified that user can see “Patient List” header.
+4. Verified that user can see table header with #, Full Name and Action.
+5. Verified that user can see one patient data which is 1, Patient1 Generic, and View button.
+6. Verified that user can see “Register New Patient” button.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. User logged in website
+2. User click on Patient List button on the dashboard.
+3. Patient redirect to Patient List page.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">patient1
+First name = Patient1
+Last name = Generic
+Ic number = 12121212121212
+Tel number = 090090091111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Logged in user should be redirect to patient list page after clicking the Patient List button on dashboard.
+2. User should be able to see search input with “Search patient” placeholder and Search button.
+3. User should be able to see “Patient List” header.
+4. User should be able to see table header with #, Full Name and Action.
+5. User should be able to see one patient data which is 1, Nur Aira Amanda Mohammad Rahimi, View button.
+6. User should be able to see Register New Patient button.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Logged in user can be redirect to Patient List page after clicking the Patient List button.
+2. User can see search input with “Search patient” placeholder and Search button.
+3. User can see “Patient List” header.
+4. User can see table header with #, Full Name and Action.
+5. User can see patient data which is 1, Patient1 Generic, View button.
+6. User can see Register New Patient button.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_patient_list_page</t>
   </si>
 </sst>
 </file>
@@ -118,6 +204,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -137,8 +224,10 @@
     <font>
       <b val="true"/>
       <sz val="10"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -200,27 +289,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -407,123 +496,221 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:G17"/>
+  <dimension ref="A2:H18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B3" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="76.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="92.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="33.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="39.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="76.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="92.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="33.6"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="E5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="F5" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="85.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="n">
+      <c r="G5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="C6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="D6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="E6" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="85.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="B6" s="4" t="s">
+      <c r="F6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="G6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="H6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="3" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="C7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="85.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="B7" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="E7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="F7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="G7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="0" t="s">
+      <c r="C8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="6"/>
+      <c r="D8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="162.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="Clinic Mangement System Functional Test Cases (http://localhost:8000)"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>